<commit_message>
Cleaned NA Values + Reset Working Environment
</commit_message>
<xml_diff>
--- a/Data/Column Selection.xlsx
+++ b/Data/Column Selection.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaizh\Desktop\control-cycle\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37D5EB85-9886-4D8D-BEA2-C47692820087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0236494B-EE54-4142-B208-EF18E26C931A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Column Selection" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="50">
   <si>
     <t>Position</t>
   </si>
@@ -166,16 +166,16 @@
     <t>Penalty Kicks PKsv</t>
   </si>
   <si>
-    <t>Penalty Kicks Save%</t>
-  </si>
-  <si>
     <t>1/3</t>
+  </si>
+  <si>
+    <t>Penalty Kicks PKA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1010,11 +1010,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1168,7 +1168,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1296,7 +1296,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1304,7 +1304,7 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1312,7 +1312,7 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -1320,7 +1320,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -1328,7 +1328,7 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1336,7 +1336,7 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1344,7 +1344,7 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1352,7 +1352,7 @@
         <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1360,7 +1360,7 @@
         <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1368,7 +1368,7 @@
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1376,7 +1376,7 @@
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -1384,7 +1384,7 @@
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1392,23 +1392,23 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>32</v>
       </c>
-      <c r="B48" t="s">
-        <v>19</v>
+      <c r="B48" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>49</v>
+      <c r="B49" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1416,7 +1416,7 @@
         <v>32</v>
       </c>
       <c r="B50" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1424,7 +1424,7 @@
         <v>32</v>
       </c>
       <c r="B51" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -1432,7 +1432,7 @@
         <v>32</v>
       </c>
       <c r="B52" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -1440,7 +1440,7 @@
         <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -1448,7 +1448,7 @@
         <v>32</v>
       </c>
       <c r="B54" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -1456,7 +1456,7 @@
         <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -1464,7 +1464,7 @@
         <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -1472,7 +1472,7 @@
         <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1480,7 +1480,7 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -1488,7 +1488,7 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1496,7 +1496,7 @@
         <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -1504,7 +1504,7 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -1512,7 +1512,7 @@
         <v>32</v>
       </c>
       <c r="B62" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -1520,7 +1520,7 @@
         <v>32</v>
       </c>
       <c r="B63" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -1528,7 +1528,7 @@
         <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -1536,7 +1536,7 @@
         <v>32</v>
       </c>
       <c r="B65" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -1544,7 +1544,7 @@
         <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
@@ -1552,15 +1552,15 @@
         <v>32</v>
       </c>
       <c r="B67" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B68" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -1568,7 +1568,7 @@
         <v>40</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
@@ -1576,7 +1576,7 @@
         <v>40</v>
       </c>
       <c r="B70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -1584,7 +1584,7 @@
         <v>40</v>
       </c>
       <c r="B71" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -1592,7 +1592,7 @@
         <v>40</v>
       </c>
       <c r="B72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -1600,7 +1600,7 @@
         <v>40</v>
       </c>
       <c r="B73" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -1608,7 +1608,7 @@
         <v>40</v>
       </c>
       <c r="B74" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -1616,7 +1616,7 @@
         <v>40</v>
       </c>
       <c r="B75" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -1624,7 +1624,7 @@
         <v>40</v>
       </c>
       <c r="B76" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -1632,23 +1632,23 @@
         <v>40</v>
       </c>
       <c r="B77" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>40</v>
       </c>
-      <c r="B78" t="s">
-        <v>19</v>
+      <c r="B78" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>40</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>49</v>
+      <c r="B79" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
@@ -1656,7 +1656,7 @@
         <v>40</v>
       </c>
       <c r="B80" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -1664,7 +1664,7 @@
         <v>40</v>
       </c>
       <c r="B81" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -1672,7 +1672,7 @@
         <v>40</v>
       </c>
       <c r="B82" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -1680,7 +1680,7 @@
         <v>40</v>
       </c>
       <c r="B83" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -1688,7 +1688,7 @@
         <v>40</v>
       </c>
       <c r="B84" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -1696,7 +1696,7 @@
         <v>40</v>
       </c>
       <c r="B85" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -1704,7 +1704,7 @@
         <v>40</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -1712,7 +1712,7 @@
         <v>40</v>
       </c>
       <c r="B87" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -1720,7 +1720,7 @@
         <v>40</v>
       </c>
       <c r="B88" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -1728,7 +1728,7 @@
         <v>40</v>
       </c>
       <c r="B89" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -1736,7 +1736,7 @@
         <v>40</v>
       </c>
       <c r="B90" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -1744,7 +1744,7 @@
         <v>40</v>
       </c>
       <c r="B91" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -1752,7 +1752,7 @@
         <v>40</v>
       </c>
       <c r="B92" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -1760,15 +1760,15 @@
         <v>40</v>
       </c>
       <c r="B93" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B94" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -1776,7 +1776,7 @@
         <v>41</v>
       </c>
       <c r="B95" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -1784,7 +1784,7 @@
         <v>41</v>
       </c>
       <c r="B96" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
@@ -1792,7 +1792,7 @@
         <v>41</v>
       </c>
       <c r="B97" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
@@ -1800,7 +1800,7 @@
         <v>41</v>
       </c>
       <c r="B98" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -1808,7 +1808,7 @@
         <v>41</v>
       </c>
       <c r="B99" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -1816,15 +1816,7 @@
         <v>41</v>
       </c>
       <c r="B100" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>41</v>
-      </c>
-      <c r="B101" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>